<commit_message>
Add combine result script - combine.py
</commit_message>
<xml_diff>
--- a/output/Result_Edgeprop.xlsx
+++ b/output/Result_Edgeprop.xlsx
@@ -1769,7 +1769,7 @@
     <t>FamilyMart Petron Setia Impian</t>
   </si>
   <si>
-    <t>Family Mart Ecohill Taipan</t>
+    <t>FamilyMart Ecohill Taipan</t>
   </si>
   <si>
     <t>FamilyMart Alamanda Shopping Centre</t>
@@ -1922,7 +1922,7 @@
     <t>FamilyMart Seksyen 15, Bangi</t>
   </si>
   <si>
-    <t>FamillyMart Malim Jaya</t>
+    <t>FamilyMart Malim Jaya</t>
   </si>
   <si>
     <t>FamilyMart Galleria @ Kotaraya</t>
@@ -4173,8 +4173,8 @@
   <sheetPr/>
   <dimension ref="A1:I1862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1834" workbookViewId="0">
-      <selection activeCell="A1854" sqref="A1854"/>
+    <sheetView tabSelected="1" topLeftCell="A888" workbookViewId="0">
+      <selection activeCell="A920" sqref="A920"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>